<commit_message>
Update examples in excel s/h
</commit_message>
<xml_diff>
--- a/LargeDeviationEx.xlsx
+++ b/LargeDeviationEx.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7050" firstSheet="7" activeTab="7"/>
   </bookViews>
@@ -14,15 +14,14 @@
     <sheet name="ex3" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
-    <sheet name="Lesign ex 1" sheetId="11" r:id="rId8"/>
-    <sheet name="Sheet3" sheetId="14" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="14" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>n</t>
   </si>
@@ -215,65 +214,17 @@
   <si>
     <t>p=.06</t>
   </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>"(2)"</t>
-  </si>
-  <si>
-    <t>"(1)"</t>
-  </si>
-  <si>
-    <t>LD Prob</t>
-  </si>
-  <si>
-    <t>I(z)</t>
-  </si>
-  <si>
-    <t>Heads or Tails An Introduction by Emmanuel Lesigne</t>
-  </si>
-  <si>
-    <t>Rate Functions</t>
-  </si>
-  <si>
-    <t>Large Deviation Probability</t>
-  </si>
-  <si>
-    <t>Rate Eqns</t>
-  </si>
-  <si>
-    <t>#1</t>
-  </si>
-  <si>
-    <t>#2</t>
-  </si>
-  <si>
-    <t>Question. What is prob that 60 head events from 100 tosses</t>
-  </si>
-  <si>
-    <t>Compute example from</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.0000000000%"/>
-    <numFmt numFmtId="166" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -307,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,18 +266,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,7 +290,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.37909033245844281"/>
-          <c:y val="1.3888888888888919E-2"/>
+          <c:y val="1.3888888888888923E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -417,24 +356,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="45205376"/>
-        <c:axId val="45206912"/>
+        <c:axId val="121382784"/>
+        <c:axId val="121384320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45205376"/>
+        <c:axId val="121382784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45206912"/>
+        <c:crossAx val="121384320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45206912"/>
+        <c:axId val="121384320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +381,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45205376"/>
+        <c:crossAx val="121382784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -455,7 +394,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -528,24 +467,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134144384"/>
-        <c:axId val="134147456"/>
+        <c:axId val="121995264"/>
+        <c:axId val="121996800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134144384"/>
+        <c:axId val="121995264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134147456"/>
+        <c:crossAx val="121996800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134147456"/>
+        <c:axId val="121996800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +492,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134144384"/>
+        <c:crossAx val="121995264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -566,7 +505,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -639,24 +578,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134183936"/>
-        <c:axId val="134210304"/>
+        <c:axId val="122324096"/>
+        <c:axId val="122325632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134183936"/>
+        <c:axId val="122324096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134210304"/>
+        <c:crossAx val="122325632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134210304"/>
+        <c:axId val="122325632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +603,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134183936"/>
+        <c:crossAx val="122324096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -677,7 +616,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -739,7 +678,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -759,7 +698,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -900,7 +839,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -920,7 +859,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1029,7 +968,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1049,7 +988,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1084,7 +1023,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1104,7 +1043,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1144,7 +1083,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1164,7 +1103,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1204,7 +1143,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1224,7 +1163,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1365,7 +1304,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1385,7 +1324,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1489,7 +1428,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1509,138 +1448,13 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>93543</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4292600" y="647700"/>
-          <a:ext cx="4603750" cy="734893"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4098" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3873500" y="1263650"/>
-          <a:ext cx="2857500" cy="317500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4104" name="Picture 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4286250" y="2209800"/>
-          <a:ext cx="2114550" cy="781050"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1933,6 +1747,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A6:N40"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
@@ -3492,6 +3307,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A5:M133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8125,6 +7941,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
@@ -8215,6 +8032,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8344,6 +8162,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="C4:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8485,6 +8304,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="C1:P104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8510,7 +8330,7 @@
       </c>
       <c r="H2">
         <f ca="1">AVERAGE(E5:E110)</f>
-        <v>0.44240000000000007</v>
+        <v>0.46669999999999995</v>
       </c>
       <c r="L2" t="s">
         <v>63</v>
@@ -8531,7 +8351,7 @@
       </c>
       <c r="H3">
         <f ca="1">STDEVP(E6:E111)</f>
-        <v>0.27862174818813362</v>
+        <v>0.29820275856503098</v>
       </c>
       <c r="K3" t="s">
         <v>0</v>
@@ -8557,26 +8377,26 @@
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E69" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.79</v>
+        <v>0.08</v>
       </c>
       <c r="G5">
         <f ca="1">$H$3/SQRT(D5)</f>
-        <v>0.27862174818813362</v>
+        <v>0.29820275856503098</v>
       </c>
       <c r="H5">
         <f ca="1">(E5-$H$2)/G5</f>
-        <v>1.2475695176720023</v>
+        <v>-1.2967686880591676</v>
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I36" ca="1" si="1">NORMSDIST(H5)</f>
-        <v>0.89390562636802606</v>
+        <v>9.7355393687597935E-2</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5">
         <f ca="1">G5*LN(G5/$L$3)+(1-G5)*LN((1-G5)/(1-$L$3))+LN(2)</f>
-        <v>0.93001326786891625</v>
+        <v>0.96620420115348615</v>
       </c>
     </row>
     <row r="6" spans="3:16">
@@ -8586,19 +8406,19 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.93</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G69" ca="1" si="2">$H$3/SQRT(D6)</f>
-        <v>0.19701532752987994</v>
+        <v>0.2108611927498682</v>
       </c>
       <c r="H6">
         <f t="shared" ref="H6:H69" ca="1" si="3">(E6-$H$2)/G6</f>
-        <v>-0.8243013476977824</v>
+        <v>2.1971800214067114</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.204884176519045</v>
+        <v>0.98599620407029798</v>
       </c>
       <c r="K6">
         <f>K5+1</f>
@@ -8606,7 +8426,7 @@
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L69" ca="1" si="4">G6*LN(G6/$L$3)+(1-G6)*LN((1-G6)/(1-$L$3))+LN(2)</f>
-        <v>0.80088036931435502</v>
+        <v>0.82011914850362921</v>
       </c>
     </row>
     <row r="7" spans="3:16">
@@ -8616,19 +8436,19 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13</v>
+        <v>0.9</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16086234131850308</v>
+        <v>0.17216744293060962</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.9420331535611342</v>
+        <v>2.516735990408113</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6066543435855349E-2</v>
+        <v>0.99407762262301524</v>
       </c>
       <c r="K7">
         <f t="shared" ref="K7:K70" si="6">K6+1</f>
@@ -8636,7 +8456,7 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="4"/>
-        <v>0.75654392144520055</v>
+        <v>0.76944100483427391</v>
       </c>
       <c r="P7">
         <f>LOG(2^11,2)</f>
@@ -8650,19 +8470,19 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.59</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.13931087409406681</v>
+        <v>0.14910137928251549</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.44791909034944211</v>
+        <v>0.8269541207018124</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32710579514964211</v>
+        <v>0.7958684669117716</v>
       </c>
       <c r="K8">
         <f t="shared" si="6"/>
@@ -8670,7 +8490,7 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.73463082698674165</v>
+        <v>0.7441331272020878</v>
       </c>
     </row>
     <row r="9" spans="3:16">
@@ -8680,19 +8500,19 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24</v>
+        <v>0.17</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12460343379169912</v>
+        <v>0.13336032784587337</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.6243533090617255</v>
+        <v>-2.2247995696508847</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2150212956842745E-2</v>
+        <v>1.3047348155656668E-2</v>
       </c>
       <c r="K9">
         <f t="shared" si="6"/>
@@ -8700,7 +8520,7 @@
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="4"/>
-        <v>0.72187557301257188</v>
+        <v>0.72924324324278078</v>
       </c>
     </row>
     <row r="10" spans="3:16">
@@ -8710,19 +8530,19 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.04</v>
+        <v>0.67</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11374685238385848</v>
+        <v>0.12174076639578199</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.5376803099749212</v>
+        <v>1.6699418446165124</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>2.018292351874118E-4</v>
+        <v>0.95253456486899313</v>
       </c>
       <c r="K10">
         <f t="shared" si="6"/>
@@ -8730,7 +8550,7 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="4"/>
-        <v>0.71372302903960205</v>
+        <v>0.71961754368395781</v>
       </c>
     </row>
     <row r="11" spans="3:16">
@@ -8740,19 +8560,19 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.09</v>
+        <v>0.76</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10530912222283753</v>
+        <v>0.11271004849092975</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.3463387839688776</v>
+        <v>2.6022524515514083</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0943140495874886E-4</v>
+        <v>0.99536931751745428</v>
       </c>
       <c r="K11">
         <f t="shared" si="6"/>
@@ -8760,7 +8580,7 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="4"/>
-        <v>0.70819023978742335</v>
+        <v>0.71300415904442838</v>
       </c>
     </row>
     <row r="12" spans="3:16">
@@ -8770,19 +8590,19 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59</v>
+        <v>0.63</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>9.8507663764939968E-2</v>
+        <v>0.1054305963749341</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4983605778348839</v>
+        <v>1.5488862399987742</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9329802035163639</v>
+        <v>0.9392954653628709</v>
       </c>
       <c r="K12">
         <f t="shared" si="6"/>
@@ -8790,7 +8610,7 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="4"/>
-        <v>0.70427835191727628</v>
+        <v>0.70826465503599723</v>
       </c>
     </row>
     <row r="13" spans="3:16">
@@ -8800,19 +8620,19 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36</v>
+        <v>0.82</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>9.2873916062711212E-2</v>
+        <v>9.9400919521676998E-2</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.88722435203831795</v>
+        <v>3.5542930759604654</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18747906203217424</v>
+        <v>0.99981050169130481</v>
       </c>
       <c r="K13">
         <f t="shared" si="6"/>
@@ -8820,7 +8640,7 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="4"/>
-        <v>0.70143137597441585</v>
+        <v>0.70476306287466706</v>
       </c>
     </row>
     <row r="14" spans="3:16">
@@ -8830,19 +8650,19 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>8.8107932993239449E-2</v>
+        <v>9.4299992161078219E-2</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.36773079221465971</v>
+        <v>-4.2067872001768372</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35653698901693431</v>
+        <v>1.2951341909706038E-5</v>
       </c>
       <c r="K14">
         <f t="shared" si="6"/>
@@ -8850,7 +8670,7 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69931639739748575</v>
+        <v>0.7021172068205821</v>
       </c>
     </row>
     <row r="15" spans="3:16">
@@ -8860,19 +8680,19 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43</v>
+        <v>0.04</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>8.4007617924811248E-2</v>
+        <v>8.9911514691740704E-2</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.14760566132345715</v>
+        <v>-4.745777017136569</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44132699347848836</v>
+        <v>1.0385372358756584E-6</v>
       </c>
       <c r="K15">
         <f t="shared" si="6"/>
@@ -8880,7 +8700,7 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69772263335933993</v>
+        <v>0.70008423941803988</v>
       </c>
     </row>
     <row r="16" spans="3:16">
@@ -8890,19 +8710,19 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.09</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>8.0431170659251539E-2</v>
+        <v>8.6083721465304811E-2</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.3813859367153878</v>
+        <v>1.0838286079163497</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8963387539190393E-6</v>
+        <v>0.86077960080726246</v>
       </c>
       <c r="K16">
         <f t="shared" si="6"/>
@@ -8910,7 +8730,7 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69651061136315184</v>
+        <v>0.69850288486257017</v>
       </c>
     </row>
     <row r="17" spans="4:12">
@@ -8920,19 +8740,19 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.67</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="2"/>
-        <v>7.727576919628705E-2</v>
+        <v>8.2706564345463654E-2</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.8191044084475205</v>
+        <v>2.4580878387212421</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2102045256539071E-7</v>
+        <v>0.99301604972304558</v>
       </c>
       <c r="K17">
         <f t="shared" si="6"/>
@@ -8940,7 +8760,7 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69558468634877257</v>
+        <v>0.69726213722691444</v>
       </c>
     </row>
     <row r="18" spans="4:12">
@@ -8950,19 +8770,19 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="2"/>
-        <v>7.4464794444571367E-2</v>
+        <v>7.9698039595801032E-2</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="3"/>
-        <v>6.5480607800905171</v>
+        <v>1.4216158963835961</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99999999997085554</v>
+        <v>0.92243110626810387</v>
       </c>
       <c r="K18">
         <f t="shared" si="6"/>
@@ -8970,7 +8790,7 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="4"/>
-        <v>0.6948773014268701</v>
+        <v>0.69628329507836662</v>
       </c>
     </row>
     <row r="19" spans="4:12">
@@ -8980,19 +8800,19 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52</v>
+        <v>0.85</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1939826041589203E-2</v>
+        <v>7.6995621181031745E-2</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0786792833657748</v>
+        <v>4.9782051773929696</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85963463799627327</v>
+        <v>0.99999967911671805</v>
       </c>
       <c r="K19">
         <f t="shared" si="6"/>
@@ -9000,7 +8820,7 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69433953939935922</v>
+        <v>0.69550915320369211</v>
       </c>
     </row>
     <row r="20" spans="4:12">
@@ -9010,19 +8830,19 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9655437047033406E-2</v>
+        <v>7.4550689641257745E-2</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9902780706880092</v>
+        <v>-6.2601701237880896</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99999969853769555</v>
+        <v>1.922788593007303E-10</v>
       </c>
       <c r="K20">
         <f t="shared" si="6"/>
@@ -9030,7 +8850,7 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69393522269823371</v>
+        <v>0.6948972387784017</v>
       </c>
     </row>
     <row r="21" spans="4:12">
@@ -9040,19 +8860,19 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.82</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>6.7575699845524764E-2</v>
+        <v>7.2324792436128479E-2</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7402705450158664</v>
+        <v>4.8849085921954982</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9590942382203036</v>
+        <v>0.99999948261571969</v>
       </c>
       <c r="K21">
         <f t="shared" si="6"/>
@@ -9060,7 +8880,7 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69363710364644826</v>
+        <v>0.69441543438699405</v>
       </c>
     </row>
     <row r="22" spans="4:12">
@@ -9070,19 +8890,19 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.21</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
-        <v>6.5671775843293326E-2</v>
+        <v>7.028706424995608E-2</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="3"/>
-        <v>6.3588961108114601</v>
+        <v>-3.6521656259125992</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99999999989839561</v>
+        <v>1.3001903675147197E-4</v>
       </c>
       <c r="K22">
         <f t="shared" si="6"/>
@@ -9090,7 +8910,7 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69342433253614377</v>
+        <v>0.69403906277299021</v>
       </c>
     </row>
     <row r="23" spans="4:12">
@@ -9100,19 +8920,19 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59</v>
+        <v>0.39</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3920212832879533E-2</v>
+        <v>6.8412404698422524E-2</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.3091287318755112</v>
+        <v>-1.1211417043167977</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9895317805873568</v>
+        <v>0.131113774595218</v>
       </c>
       <c r="K23">
         <f t="shared" si="6"/>
@@ -9120,7 +8940,7 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69328073221408859</v>
+        <v>0.69374889584502886</v>
       </c>
     </row>
     <row r="24" spans="4:12">
@@ -9130,19 +8950,19 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.7</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>6.2301716895849561E-2</v>
+        <v>6.6680163922936686E-2</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="3"/>
-        <v>7.0238834787095916</v>
+        <v>3.4987916386892581</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99999999999892109</v>
+        <v>0.99976631417215656</v>
       </c>
       <c r="K24">
         <f t="shared" si="6"/>
@@ -9150,7 +8970,7 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69319359610353359</v>
+        <v>0.69352976462751648</v>
       </c>
     </row>
     <row r="25" spans="4:12">
@@ -9160,19 +8980,19 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77</v>
+        <v>0.12</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>6.0800250063478452E-2</v>
+        <v>6.5073176836614066E-2</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3881357339479594</v>
+        <v>-5.327848075874571</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99999996440386052</v>
+        <v>4.9691598314727132E-8</v>
       </c>
       <c r="K25">
         <f t="shared" si="6"/>
@@ -9180,7 +9000,7 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69315283439409991</v>
+        <v>0.6933695696606208</v>
       </c>
     </row>
     <row r="26" spans="4:12">
@@ -9190,19 +9010,19 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>5.9402356305962592E-2</v>
+        <v>6.3577041745283752E-2</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="3"/>
-        <v>0.80131501442177644</v>
+        <v>1.6248003550379562</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78852534956574871</v>
+        <v>0.94789744730583991</v>
       </c>
       <c r="K26">
         <f t="shared" si="6"/>
@@ -9210,7 +9030,7 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69315035692335436</v>
+        <v>0.6932585641300989</v>
       </c>
     </row>
     <row r="27" spans="4:12">
@@ -9220,19 +9040,19 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12</v>
+        <v>0.26</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8096650567006518E-2</v>
+        <v>6.2179573472390774E-2</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.5493732745944779</v>
+        <v>-3.3242428092849448</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4334773705920217E-8</v>
+        <v>4.4329483898153388E-4</v>
       </c>
       <c r="K27">
         <f t="shared" si="6"/>
@@ -9240,7 +9060,7 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69317962013215983</v>
+        <v>0.69318882639864021</v>
       </c>
     </row>
     <row r="28" spans="4:12">
@@ -9250,19 +9070,19 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93</v>
+        <v>0.2</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6873426191929241E-2</v>
+        <v>6.0870383197890995E-2</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="3"/>
-        <v>8.5734240514103934</v>
+        <v>-4.3814411210941815</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5.8948452723583955E-6</v>
       </c>
       <c r="K28">
         <f t="shared" si="6"/>
@@ -9270,7 +9090,7 @@
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69323528976540338</v>
+        <v>0.69315386639604648</v>
       </c>
     </row>
     <row r="29" spans="4:12">
@@ -9280,19 +9100,19 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34</v>
+        <v>0.96</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5724349637626722E-2</v>
+        <v>5.9640551713006196E-2</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.8376167809207871</v>
+        <v>8.2712179185361716</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3059447147213206E-2</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="K29">
         <f t="shared" si="6"/>
@@ -9300,7 +9120,7 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69331298652841256</v>
+        <v>0.69314832812503135</v>
       </c>
     </row>
     <row r="30" spans="4:12">
@@ -9310,19 +9130,19 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53</v>
+        <v>0.02</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>5.4642220420101098E-2</v>
+        <v>5.8482372497318885E-2</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="3"/>
-        <v>1.6031559355844691</v>
+        <v>-7.6381990149335826</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94554988440554621</v>
+        <v>1.1014059615844397E-14</v>
       </c>
       <c r="K30">
         <f t="shared" si="6"/>
@@ -9330,7 +9150,7 @@
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69340909205998258</v>
+        <v>0.6931677621826704</v>
       </c>
     </row>
     <row r="31" spans="4:12">
@@ -9340,19 +9160,19 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73</v>
+        <v>0.86</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>5.3620780439501026E-2</v>
+        <v>5.7389147643536538E-2</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3635922051617984</v>
+        <v>6.8532120818890663</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99999995920851203</v>
+        <v>0.99999999999638955</v>
       </c>
       <c r="K31">
         <f t="shared" si="6"/>
@@ -9360,7 +9180,7 @@
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69352059934077881</v>
+        <v>0.69320844995967468</v>
       </c>
     </row>
     <row r="32" spans="4:12">
@@ -9370,19 +9190,19 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="2"/>
-        <v>5.2654561111418766E-2</v>
+        <v>5.6355024245464874E-2</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.42541423814360463</v>
+        <v>-0.47378206925620492</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.335267364228927</v>
+        <v>0.31782766116343031</v>
       </c>
       <c r="K32">
         <f t="shared" si="6"/>
@@ -9390,7 +9210,7 @@
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69364499623343101</v>
+        <v>0.6932672664446633</v>
       </c>
     </row>
     <row r="33" spans="4:12">
@@ -9400,19 +9220,19 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.86</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="2"/>
-        <v>5.173875975327686E-2</v>
+        <v>5.5374862097063181E-2</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.1388460174620727</v>
+        <v>7.1025007576652515</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="1"/>
-        <v>8.4807275698550733E-4</v>
+        <v>0.99999999999938738</v>
       </c>
       <c r="K33">
         <f t="shared" si="6"/>
@@ -9420,7 +9240,7 @@
       </c>
       <c r="L33">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69378017400078629</v>
+        <v>0.69334157218880255</v>
       </c>
     </row>
     <row r="34" spans="4:12">
@@ -9430,19 +9250,19 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0869138831388307E-2</v>
+        <v>5.4444125858778114E-2</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="3"/>
-        <v>9.5853794894426478</v>
+        <v>-7.2863691673367068</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>1.5920985620244997E-13</v>
       </c>
       <c r="K34">
         <f t="shared" si="6"/>
@@ -9450,7 +9270,7 @@
       </c>
       <c r="L34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69392435484839243</v>
+        <v>0.69342912752305663</v>
       </c>
     </row>
     <row r="35" spans="4:12">
@@ -9460,19 +9280,19 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>0.62</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0041943234557767E-2</v>
+        <v>5.3558796517289828E-2</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="3"/>
-        <v>-8.2410868432304714</v>
+        <v>2.8622749196859156</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>8.532665116848064E-17</v>
+        <v>0.99789694054750111</v>
       </c>
       <c r="K35">
         <f t="shared" si="6"/>
@@ -9480,7 +9300,7 @@
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69407603409390128</v>
+        <v>0.69352802391807244</v>
       </c>
     </row>
     <row r="36" spans="4:12">
@@ -9490,19 +9310,19 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="2"/>
-        <v>4.9253831882469984E-2</v>
+        <v>5.271529818746705E-2</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="3"/>
-        <v>0.56036249252361348</v>
+        <v>-0.8858908439429598</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71238389514986733</v>
+        <v>0.18783817523896318</v>
       </c>
       <c r="K36">
         <f t="shared" si="6"/>
@@ -9510,7 +9330,7 @@
       </c>
       <c r="L36">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69423393368141018</v>
+        <v>0.69363662866661524</v>
       </c>
     </row>
     <row r="37" spans="4:12">
@@ -9520,19 +9340,19 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8501820822869003E-2</v>
+        <v>5.1910437210523491E-2</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.3483279028449817</v>
+        <v>0.64148949208328654</v>
       </c>
       <c r="I37">
         <f t="shared" ref="I37:I68" ca="1" si="7">NORMSDIST(H37)</f>
-        <v>4.0650378457485203E-4</v>
+        <v>0.7393976470932595</v>
       </c>
       <c r="K37">
         <f t="shared" si="6"/>
@@ -9540,7 +9360,7 @@
       </c>
       <c r="L37">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69439696456716193</v>
+        <v>0.69375354000471301</v>
       </c>
     </row>
     <row r="38" spans="4:12">
@@ -9550,19 +9370,19 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95</v>
+        <v>0.47</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="2"/>
-        <v>4.778323560419729E-2</v>
+        <v>5.1141351179495968E-2</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="3"/>
-        <v>10.62297254636754</v>
+        <v>6.452703974163064E-2</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0.52572471131457377</v>
       </c>
       <c r="K38">
         <f t="shared" si="6"/>
@@ -9570,7 +9390,7 @@
       </c>
       <c r="L38">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69456419609525899</v>
+        <v>0.6938775504745055</v>
       </c>
     </row>
     <row r="39" spans="4:12">
@@ -9580,19 +9400,19 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="2"/>
-        <v>4.7095671188219695E-2</v>
+        <v>5.0405466034603302E-2</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.9963048168774877</v>
+        <v>-7.671787018783454</v>
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0092898296650988E-9</v>
+        <v>8.480821393998759E-15</v>
       </c>
       <c r="K39">
         <f t="shared" si="6"/>
@@ -9600,7 +9420,7 @@
       </c>
       <c r="L39">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69473483092027455</v>
+        <v>0.69400761684074908</v>
       </c>
     </row>
     <row r="40" spans="4:12">
@@ -9610,19 +9430,19 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="2"/>
-        <v>4.6436958031355606E-2</v>
+        <v>4.9700459760838499E-2</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.4204858536190992</v>
+        <v>-2.5492721920418382</v>
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="7"/>
-        <v>7.7498911804467774E-3</v>
+        <v>5.3974005513974799E-3</v>
       </c>
       <c r="K40">
         <f t="shared" si="6"/>
@@ -9630,7 +9450,7 @@
       </c>
       <c r="L40">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69490818436095758</v>
+        <v>0.69414283525359799</v>
       </c>
     </row>
     <row r="41" spans="4:12">
@@ -9640,19 +9460,19 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43</v>
+        <v>0.72</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5805133243377434E-2</v>
+        <v>4.9024231519755053E-2</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.27071201679765633</v>
+        <v>5.1668326488285485</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="7"/>
-        <v>0.39330626687370618</v>
+        <v>0.9999998809528674</v>
       </c>
       <c r="K41">
         <f t="shared" si="6"/>
@@ -9660,7 +9480,7 @@
       </c>
       <c r="L41">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69508366731584525</v>
+        <v>0.69428242063751311</v>
       </c>
     </row>
     <row r="42" spans="4:12">
@@ -9670,19 +9490,19 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16</v>
+        <v>0.68</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5198415949016503E-2</v>
+        <v>4.8374875279532999E-2</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="3"/>
-        <v>-6.2480065743575022</v>
+        <v>4.4093136936777908</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="7"/>
-        <v>2.0786209088215087E-10</v>
+        <v>0.99999481506377352</v>
       </c>
       <c r="K42">
         <f t="shared" si="6"/>
@@ -9690,7 +9510,7 @@
       </c>
       <c r="L42">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69526077205893744</v>
+        <v>0.6944256895046601</v>
       </c>
     </row>
     <row r="43" spans="4:12">
@@ -9700,19 +9520,19 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67</v>
+        <v>0.62</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="2"/>
-        <v>4.461518614731172E-2</v>
+        <v>4.7750657188602545E-2</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="3"/>
-        <v>5.1014020035353811</v>
+        <v>3.2104270187215507</v>
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="7"/>
-        <v>0.99999983142671089</v>
+        <v>0.99933731040222407</v>
       </c>
       <c r="K43">
         <f t="shared" si="6"/>
@@ -9720,7 +9540,7 @@
       </c>
       <c r="L43">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69543906037701808</v>
+        <v>0.69457204555868346</v>
       </c>
     </row>
     <row r="44" spans="4:12">
@@ -9730,19 +9550,19 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="2"/>
-        <v>4.4053966496619724E-2</v>
+        <v>4.714999608053911E-2</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="3"/>
-        <v>-10.042228547886728</v>
+        <v>-5.020148879666535</v>
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="7"/>
-        <v>4.9701302246231352E-24</v>
+        <v>2.5815723369853674E-7</v>
       </c>
       <c r="K44">
         <f t="shared" si="6"/>
@@ -9750,7 +9570,7 @@
       </c>
       <c r="L44">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69561815362080326</v>
+        <v>0.69472096758412172</v>
       </c>
     </row>
     <row r="45" spans="4:12">
@@ -9760,19 +9580,19 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>0.67</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3513406558520741E-2</v>
+        <v>4.6571446610660636E-2</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.97441233296631735</v>
+        <v>4.3653357324198483</v>
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="7"/>
-        <v>0.16492592416435836</v>
+        <v>0.99999365361712811</v>
       </c>
       <c r="K45">
         <f t="shared" si="6"/>
@@ -9780,7 +9600,7 @@
       </c>
       <c r="L45">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69579772432798059</v>
+        <v>0.69487199921733001</v>
       </c>
     </row>
     <row r="46" spans="4:12">
@@ -9790,19 +9610,19 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.17</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2992269117723428E-2</v>
+        <v>4.6013684614521176E-2</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="3"/>
-        <v>6.4569748398220783</v>
+        <v>-6.4480817497142198</v>
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="7"/>
-        <v>0.99999999994659172</v>
+        <v>5.663733230566521E-11</v>
       </c>
       <c r="K46">
         <f t="shared" si="6"/>
@@ -9810,7 +9630,7 @@
       </c>
       <c r="L46">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69597748914331814</v>
+        <v>0.69502474027351391</v>
       </c>
     </row>
     <row r="47" spans="4:12">
@@ -9820,19 +9640,19 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="0"/>
-        <v>0.01</v>
+        <v>0.99</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2489418262261366E-2</v>
+        <v>4.5475494350406105E-2</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="3"/>
-        <v>-10.176651450746101</v>
+        <v>11.507296566536983</v>
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="7"/>
-        <v>1.2604353131527306E-24</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <f t="shared" si="6"/>
@@ -9840,7 +9660,7 @@
       </c>
       <c r="L47">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69615720281379356</v>
+        <v>0.69517883936650171</v>
       </c>
     </row>
     <row r="48" spans="4:12">
@@ -9850,19 +9670,19 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45</v>
+        <v>0.13</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2003808962405624E-2</v>
+        <v>4.4955757345870352E-2</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1809359719448804</v>
+        <v>-7.4895857589401569</v>
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="7"/>
-        <v>0.5717910833559674</v>
+        <v>3.4545663677562868E-14</v>
       </c>
       <c r="K48">
         <f t="shared" si="6"/>
@@ -9870,7 +9690,7 @@
       </c>
       <c r="L48">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69633665307844617</v>
+        <v>0.69533398760698173</v>
       </c>
     </row>
     <row r="49" spans="4:12">
@@ -9880,19 +9700,19 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="2"/>
-        <v>4.1534477930566374E-2</v>
+        <v>4.4453442615291126E-2</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.4284769448180299</v>
+        <v>-2.8501729572777244</v>
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="7"/>
-        <v>3.0348904364752016E-4</v>
+        <v>2.1847730528247178E-3</v>
       </c>
       <c r="K49">
         <f t="shared" si="6"/>
@@ -9900,7 +9720,7 @@
       </c>
       <c r="L49">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69651565630584344</v>
+        <v>0.69548991320407993</v>
       </c>
     </row>
     <row r="50" spans="4:12">
@@ -9910,19 +9730,19 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84</v>
+        <v>0.39</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="2"/>
-        <v>4.1080535580155585E-2</v>
+        <v>4.3967598053614672E-2</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="3"/>
-        <v>9.6785495706162372</v>
+        <v>-1.7444664570138886</v>
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>4.0538892734229837E-2</v>
       </c>
       <c r="K50">
         <f t="shared" si="6"/>
@@ -9930,7 +9750,7 @@
       </c>
       <c r="L50">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69669405375861049</v>
+        <v>0.69564637682646946</v>
       </c>
     </row>
     <row r="51" spans="4:12">
@@ -9940,19 +9760,19 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.78</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0641158930590629E-2</v>
+        <v>4.3497342842736951E-2</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="3"/>
-        <v>-8.1789006206169574</v>
+        <v>7.2027388232132878</v>
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="7"/>
-        <v>1.4322261162507054E-16</v>
+        <v>0.9999999999997049</v>
       </c>
       <c r="K51">
         <f t="shared" si="6"/>
@@ -9960,7 +9780,7 @@
       </c>
       <c r="L51">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69687170838578527</v>
+        <v>0.6958031676044254</v>
       </c>
     </row>
     <row r="52" spans="4:12">
@@ -9970,19 +9790,19 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0215585329625769E-2</v>
+        <v>4.3041860732652405E-2</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="3"/>
-        <v>4.6648581255834642</v>
+        <v>-9.2166089766434158</v>
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="7"/>
-        <v>0.99999845584969538</v>
+        <v>1.5332218468283391E-20</v>
       </c>
       <c r="K52">
         <f t="shared" si="6"/>
@@ -9990,7 +9810,7 @@
       </c>
       <c r="L52">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69704850206100111</v>
+        <v>0.69596009967462746</v>
       </c>
     </row>
     <row r="53" spans="4:12">
@@ -10000,19 +9820,19 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9803106884019092E-2</v>
+        <v>4.2600394080718709E-2</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="3"/>
-        <v>-11.114710248350569</v>
+        <v>-6.2605054660916988</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="7"/>
-        <v>5.319772830880276E-29</v>
+        <v>1.9186581095694664E-10</v>
       </c>
       <c r="K53">
         <f t="shared" si="6"/>
@@ -10020,7 +9840,7 @@
       </c>
       <c r="L53">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69722433319844579</v>
+        <v>0.69611700918607611</v>
       </c>
     </row>
     <row r="54" spans="4:12">
@@ -10030,19 +9850,19 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>0.37</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9403065505975984E-2</v>
+        <v>4.2172238549973644E-2</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5072635268203838</v>
+        <v>-2.2929776394348025</v>
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="7"/>
-        <v>0.99999671654734068</v>
+        <v>1.0924646166150187E-2</v>
       </c>
       <c r="K54">
         <f t="shared" si="6"/>
@@ -10050,7 +9870,7 @@
       </c>
       <c r="L54">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69739911468994553</v>
+        <v>0.6962737516990064</v>
       </c>
     </row>
     <row r="55" spans="4:12">
@@ -10060,19 +9880,19 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>0.42</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9014848496491068E-2</v>
+        <v>4.1756738382082589E-2</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="3"/>
-        <v>9.165741090399516</v>
+        <v>-1.1183823691564587</v>
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0.13170186052930966</v>
       </c>
       <c r="K55">
         <f t="shared" si="6"/>
@@ -10080,7 +9900,7 @@
       </c>
       <c r="L55">
         <f t="shared" ca="1" si="4"/>
-        <v>0.6975727721158087</v>
+        <v>0.69643019991975319</v>
       </c>
     </row>
     <row r="56" spans="4:12">
@@ -10090,19 +9910,19 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36</v>
+        <v>0.78</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8637884598143525E-2</v>
+        <v>4.1353282172731827E-2</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.132621929409646</v>
+        <v>7.5761821925367929</v>
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="7"/>
-        <v>1.647787645261789E-2</v>
+        <v>0.99999999999998224</v>
       </c>
       <c r="K56">
         <f t="shared" si="6"/>
@@ -10110,7 +9930,7 @@
       </c>
       <c r="L56">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69774524218972589</v>
+        <v>0.69658624172363115</v>
       </c>
     </row>
     <row r="57" spans="4:12">
@@ -10120,19 +9940,19 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.13</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8271640459491663E-2</v>
+        <v>4.0961299087547413E-2</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.6304500996252536</v>
+        <v>-8.2199541396468945</v>
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="7"/>
-        <v>5.1503201733697601E-2</v>
+        <v>1.017905073183954E-16</v>
       </c>
       <c r="K57">
         <f t="shared" si="6"/>
@@ -10140,7 +9960,7 @@
       </c>
       <c r="L57">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69791647140431134</v>
+        <v>0.69674177842541718</v>
       </c>
     </row>
     <row r="58" spans="4:12">
@@ -10150,19 +9970,19 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7915617461286154E-2</v>
+        <v>4.0580255465260659E-2</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.1182727023578789</v>
+        <v>13.141859110683511</v>
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="7"/>
-        <v>0.13172527091819397</v>
+        <v>1</v>
       </c>
       <c r="K58">
         <f t="shared" si="6"/>
@@ -10170,7 +9990,7 @@
       </c>
       <c r="L58">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69808641484908684</v>
+        <v>0.69689672326325458</v>
       </c>
     </row>
     <row r="59" spans="4:12">
@@ -10180,19 +10000,19 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7569348861541549E-2</v>
+        <v>4.0209651762140655E-2</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3963857204514825</v>
+        <v>-9.8657904909664573</v>
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="7"/>
-        <v>0.9996585896830873</v>
+        <v>2.9285628851494397E-23</v>
       </c>
       <c r="K59">
         <f t="shared" si="6"/>
@@ -10200,7 +10020,7 @@
       </c>
       <c r="L59">
         <f t="shared" ca="1" si="4"/>
-        <v>0.6982550351770469</v>
+        <v>0.69705100006698018</v>
       </c>
     </row>
     <row r="60" spans="4:12">
@@ -10210,19 +10030,19 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>0.47</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7232397222285683E-2</v>
+        <v>3.9849019797900516E-2</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="3"/>
-        <v>4.7700393541594561</v>
+        <v>8.2812576488365444E-2</v>
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="7"/>
-        <v>0.99999907905008156</v>
+        <v>0.53299971555636116</v>
       </c>
       <c r="K60">
         <f t="shared" si="6"/>
@@ -10230,7 +10050,7 @@
       </c>
       <c r="L60">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69842230169953501</v>
+        <v>0.69720454208620997</v>
       </c>
     </row>
     <row r="61" spans="4:12">
@@ -10240,19 +10060,19 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>0.77</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6904352085721175E-2</v>
+        <v>3.9497920268543867E-2</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="3"/>
-        <v>12.399621565963001</v>
+        <v>7.6788853169453608</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0.99999999999999201</v>
       </c>
       <c r="K61">
         <f t="shared" si="6"/>
@@ -10260,7 +10080,7 @@
       </c>
       <c r="L61">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69858818959218716</v>
+        <v>0.69735729095713406</v>
       </c>
     </row>
     <row r="62" spans="4:12">
@@ -10270,19 +10090,19 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19</v>
+        <v>0.48</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6584827871723694E-2</v>
+        <v>3.9155940496103291E-2</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="3"/>
-        <v>-6.8990347825328788</v>
+        <v>0.33966748931298479</v>
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="7"/>
-        <v>2.6178526100366037E-12</v>
+        <v>0.63294652633039461</v>
       </c>
       <c r="K62">
         <f t="shared" si="6"/>
@@ -10290,7 +10110,7 @@
       </c>
       <c r="L62">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69875267919722039</v>
+        <v>0.69750919579001536</v>
       </c>
     </row>
     <row r="63" spans="4:12">
@@ -10300,19 +10120,19 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35</v>
+        <v>0.98</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6273461972186456E-2</v>
+        <v>3.882269238905893E-2</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.5473168254756051</v>
+        <v>13.221648690822358</v>
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="7"/>
-        <v>5.4277413363994498E-3</v>
+        <v>1</v>
       </c>
       <c r="K63">
         <f t="shared" si="6"/>
@@ -10320,7 +10140,7 @@
       </c>
       <c r="L63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69891575540946926</v>
+        <v>0.69766021236195586</v>
       </c>
     </row>
     <row r="64" spans="4:12">
@@ -10330,19 +10150,19 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5969913020794601E-2</v>
+        <v>3.8497810590515873E-2</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.3489147968962705</v>
+        <v>-6.6679116568576822</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="7"/>
-        <v>4.424159143267497E-8</v>
+        <v>1.2973444006835868E-11</v>
       </c>
       <c r="K64">
         <f t="shared" si="6"/>
@@ -10350,7 +10170,7 @@
       </c>
       <c r="L64">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69907740713536393</v>
+        <v>0.69781030240164665</v>
       </c>
     </row>
     <row r="65" spans="4:12">
@@ -10360,19 +10180,19 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24</v>
+        <v>0.11</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5673859319457643E-2</v>
+        <v>3.8180950794049241E-2</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.6736221945463789</v>
+        <v>-9.3423550902140988</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="7"/>
-        <v>6.9904645377973159E-9</v>
+        <v>4.7107367146367129E-21</v>
       </c>
       <c r="K65">
         <f t="shared" si="6"/>
@@ -10380,7 +10200,7 @@
       </c>
       <c r="L65">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69923762681556068</v>
+        <v>0.69795943295466567</v>
       </c>
     </row>
     <row r="66" spans="4:12">
@@ -10390,15 +10210,15 @@
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5384997404908067E-2</v>
+        <v>3.7871788209566076E-2</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="3"/>
-        <v>10.105977850104326</v>
+        <v>11.441234240176501</v>
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="7"/>
@@ -10410,7 +10230,7 @@
       </c>
       <c r="L66">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69939641000322039</v>
+        <v>0.69810757581943661</v>
       </c>
     </row>
     <row r="67" spans="4:12">
@@ -10420,19 +10240,19 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.72</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5103040740945841E-2</v>
+        <v>3.7570016163643249E-2</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="3"/>
-        <v>15.03003696726997</v>
+        <v>6.7420785473369076</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0.99999999999219313</v>
       </c>
       <c r="K67">
         <f t="shared" si="6"/>
@@ -10440,7 +10260,7 @@
       </c>
       <c r="L67">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69955375499101857</v>
+        <v>0.69825470704528914</v>
       </c>
     </row>
     <row r="68" spans="4:12">
@@ -10450,15 +10270,15 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92</v>
+        <v>0.85</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4827718523516703E-2</v>
+        <v>3.7275344820628872E-2</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="3"/>
-        <v>13.713215227621365</v>
+        <v>10.282936397891472</v>
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="7"/>
@@ -10470,7 +10290,7 @@
       </c>
       <c r="L68">
         <f t="shared" ca="1" si="4"/>
-        <v>0.6997096624809036</v>
+        <v>0.69840080648520164</v>
       </c>
     </row>
     <row r="69" spans="4:12">
@@ -10480,19 +10300,19 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.91</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4558774587296427E-2</v>
+        <v>3.6987500012383427E-2</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="3"/>
-        <v>7.4539680030984634</v>
+        <v>11.985130107511541</v>
       </c>
       <c r="I69">
         <f t="shared" ref="I69:I100" ca="1" si="8">NORMSDIST(H69)</f>
-        <v>0.9999999999999547</v>
+        <v>1</v>
       </c>
       <c r="K69">
         <f t="shared" si="6"/>
@@ -10500,7 +10320,7 @@
       </c>
       <c r="L69">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69986413529141978</v>
+        <v>0.698545857396766</v>
       </c>
     </row>
     <row r="70" spans="4:12">
@@ -10510,19 +10330,19 @@
       </c>
       <c r="E70">
         <f t="shared" ref="E70:E104" ca="1" si="9">RANDBETWEEN(0,100)/100</f>
-        <v>0.66</v>
+        <v>0.44</v>
       </c>
       <c r="G70">
         <f t="shared" ref="G70:G104" ca="1" si="10">$H$3/SQRT(D70)</f>
-        <v>3.4295966403745562E-2</v>
+        <v>3.6706222165919643E-2</v>
       </c>
       <c r="H70">
         <f t="shared" ref="H70:H104" ca="1" si="11">(E70-$H$2)/G70</f>
-        <v>6.344769453011688</v>
+        <v>-0.72739711211114233</v>
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="8"/>
-        <v>0.99999999988862065</v>
+        <v>0.23349136154554373</v>
       </c>
       <c r="K70">
         <f t="shared" si="6"/>
@@ -10530,7 +10350,7 @@
       </c>
       <c r="L70">
         <f t="shared" ref="L70:L104" ca="1" si="12">G70*LN(G70/$L$3)+(1-G70)*LN((1-G70)/(1-$L$3))+LN(2)</f>
-        <v>0.70001717809807851</v>
+        <v>0.69868984608575391</v>
       </c>
     </row>
     <row r="71" spans="4:12">
@@ -10540,19 +10360,19 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="9"/>
-        <v>0.15</v>
+        <v>0.39</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="10"/>
-        <v>3.4039064161726675E-2</v>
+        <v>3.6431265319407269E-2</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="11"/>
-        <v>-8.5901304046065103</v>
+        <v>-2.1053345067084765</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="8"/>
-        <v>4.3435336505697075E-18</v>
+        <v>1.7631100206191075E-2</v>
       </c>
       <c r="K71">
         <f t="shared" ref="K71:K104" si="14">K70+1</f>
@@ -10560,7 +10380,7 @@
       </c>
       <c r="L71">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70016879720286129</v>
+        <v>0.69883276158737651</v>
       </c>
     </row>
     <row r="72" spans="4:12">
@@ -10570,19 +10390,19 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="9"/>
-        <v>0.17</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3787849922762382E-2</v>
+        <v>3.616239621806424E-2</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="11"/>
-        <v>-8.0620696677265684</v>
+        <v>-5.1628215916382629</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="8"/>
-        <v>3.750671346787803E-16</v>
+        <v>1.2162748111026779E-7</v>
       </c>
       <c r="K72">
         <f t="shared" si="14"/>
@@ -10590,7 +10410,7 @@
       </c>
       <c r="L72">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7003190003294274</v>
+        <v>0.6989745953809442</v>
       </c>
     </row>
     <row r="73" spans="4:12">
@@ -10600,19 +10420,19 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="9"/>
-        <v>0.27</v>
+        <v>0.79</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3542116843876833E-2</v>
+        <v>3.5899393482380922E-2</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="11"/>
-        <v>-5.1398067928283409</v>
+        <v>9.0057231791025281</v>
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="8"/>
-        <v>1.3751055503854658E-7</v>
+        <v>1</v>
       </c>
       <c r="K73">
         <f t="shared" si="14"/>
@@ -10620,7 +10440,7 @@
       </c>
       <c r="L73">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70046779644103918</v>
+        <v>0.69911534113416873</v>
       </c>
     </row>
     <row r="74" spans="4:12">
@@ -10630,19 +10450,19 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="9"/>
-        <v>0.04</v>
+        <v>0.95</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3301668461722056E-2</v>
+        <v>3.5642046841936191E-2</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="11"/>
-        <v>-12.083478654005903</v>
+        <v>13.559827305747</v>
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="8"/>
-        <v>6.4569171377611377E-34</v>
+        <v>1</v>
       </c>
       <c r="K74">
         <f t="shared" si="14"/>
@@ -10650,7 +10470,7 @@
       </c>
       <c r="L74">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7006151955785862</v>
+        <v>0.69925499447380546</v>
       </c>
     </row>
     <row r="75" spans="4:12">
@@ -10660,19 +10480,19 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="9"/>
-        <v>0.27</v>
+        <v>0.95</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3066318032358342E-2</v>
+        <v>3.5390156428778873E-2</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="11"/>
-        <v>-5.2137646481017716</v>
+        <v>13.65633975008333</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="8"/>
-        <v>9.2523107999992081E-8</v>
+        <v>1</v>
       </c>
       <c r="K75">
         <f t="shared" si="14"/>
@@ -10680,7 +10500,7 @@
       </c>
       <c r="L75">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70076120871641867</v>
+        <v>0.69939355277973836</v>
       </c>
     </row>
     <row r="76" spans="4:12">
@@ -10690,19 +10510,19 @@
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="9"/>
-        <v>0.96</v>
+        <v>0.32</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2835887921646663E-2</v>
+        <v>3.514353212497804E-2</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="11"/>
-        <v>15.76324055055561</v>
+        <v>-4.1743100687290866</v>
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.4944522569448893E-5</v>
       </c>
       <c r="K76">
         <f t="shared" si="14"/>
@@ -10710,7 +10530,7 @@
       </c>
       <c r="L76">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7009058476339759</v>
+        <v>0.69953101499995096</v>
       </c>
     </row>
     <row r="77" spans="4:12">
@@ -10720,19 +10540,19 @@
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="9"/>
-        <v>0.36</v>
+        <v>0.12</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2610209041730571E-2</v>
+        <v>3.4901992959501978E-2</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="11"/>
-        <v>-2.5268160622507696</v>
+        <v>-9.9335301683857509</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="8"/>
-        <v>5.7550884094499377E-3</v>
+        <v>1.4876569712946097E-23</v>
       </c>
       <c r="K77">
         <f t="shared" si="14"/>
@@ -10740,7 +10560,7 @@
       </c>
       <c r="L77">
         <f t="shared" ca="1" si="12"/>
-        <v>0.701049124801437</v>
+        <v>0.69966738148413343</v>
       </c>
     </row>
     <row r="78" spans="4:12">
@@ -10750,19 +10570,19 @@
       </c>
       <c r="E78">
         <f t="shared" ca="1" si="9"/>
-        <v>0.52</v>
+        <v>0.04</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2389120329545544E-2</v>
+        <v>3.4665366550078083E-2</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="11"/>
-        <v>2.3958662418260483</v>
+        <v>-12.309115479381505</v>
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="8"/>
-        <v>0.99170943003385681</v>
+        <v>4.0452492692540485E-35</v>
       </c>
       <c r="K78">
         <f t="shared" si="14"/>
@@ -10770,7 +10590,7 @@
       </c>
       <c r="L78">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70119105327784226</v>
+        <v>0.69980265383393636</v>
       </c>
     </row>
     <row r="79" spans="4:12">
@@ -10780,19 +10600,19 @@
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="9"/>
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2172468263700613E-2</v>
+        <v>3.443348858612192E-2</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="11"/>
-        <v>-7.5343923883357711</v>
+        <v>-7.4549518663485159</v>
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="8"/>
-        <v>2.4530695384112867E-14</v>
+        <v>4.4950322631021815E-14</v>
       </c>
       <c r="K79">
         <f t="shared" si="14"/>
@@ -10800,7 +10620,7 @@
       </c>
       <c r="L79">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70133164662030378</v>
+        <v>0.69993683476811075</v>
       </c>
     </row>
     <row r="80" spans="4:12">
@@ -10810,19 +10630,19 @@
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="9"/>
-        <v>0.99</v>
+        <v>0.16</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1960106416439767E-2</v>
+        <v>3.4206202349211262E-2</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="11"/>
-        <v>17.133860346545131</v>
+        <v>-8.9662101881085299</v>
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.534460186435585E-19</v>
       </c>
       <c r="K80">
         <f t="shared" si="14"/>
@@ -10830,7 +10650,7 @@
       </c>
       <c r="L80">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70147091880309986</v>
+        <v>0.700069928000977</v>
       </c>
     </row>
     <row r="81" spans="4:12">
@@ -10840,19 +10660,19 @@
       </c>
       <c r="E81">
         <f t="shared" ca="1" si="9"/>
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1751895037711794E-2</v>
+        <v>3.3983358267925166E-2</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="11"/>
-        <v>-9.5238410066813</v>
+        <v>-9.0250056389946458</v>
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="8"/>
-        <v>8.3446876024016847E-22</v>
+        <v>8.9843058327933809E-20</v>
       </c>
       <c r="K81">
         <f t="shared" si="14"/>
@@ -10860,7 +10680,7 @@
       </c>
       <c r="L81">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70160888414557421</v>
+        <v>0.70020193813284004</v>
       </c>
     </row>
     <row r="82" spans="4:12">
@@ -10870,19 +10690,19 @@
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="9"/>
-        <v>0.25</v>
+        <v>0.06</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1547700668664233E-2</v>
+        <v>3.3764813504175019E-2</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="11"/>
-        <v>-6.0987012023702745</v>
+        <v>-12.045083558649347</v>
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="8"/>
-        <v>5.3466870085138565E-10</v>
+        <v>1.029338492021202E-33</v>
       </c>
       <c r="K82">
         <f t="shared" si="14"/>
@@ -10890,7 +10710,7 @@
       </c>
       <c r="L82">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70174555724789522</v>
+        <v>0.7003328705511237</v>
       </c>
     </row>
     <row r="83" spans="4:12">
@@ -10900,19 +10720,19 @@
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="9"/>
-        <v>0.55000000000000004</v>
+        <v>0.23</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1347395782132643E-2</v>
+        <v>3.355043156842806E-2</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4325020409296556</v>
+        <v>-7.0550508275053483</v>
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="8"/>
-        <v>0.99970098030965837</v>
+        <v>8.6268821849606162E-13</v>
       </c>
       <c r="K83">
         <f t="shared" si="14"/>
@@ -10920,7 +10740,7 @@
       </c>
       <c r="L83">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7018809529338319</v>
+        <v>0.70046273134113035</v>
       </c>
     </row>
     <row r="84" spans="4:12">
@@ -10930,19 +10750,19 @@
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1150858447924781E-2</v>
+        <v>3.3340081961468343E-2</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="11"/>
-        <v>5.0592506226902705</v>
+        <v>6.0977654534550068</v>
       </c>
       <c r="I84">
         <f t="shared" ca="1" si="8"/>
-        <v>0.99999978954632551</v>
+        <v>0.99999999946219298</v>
       </c>
       <c r="K84">
         <f t="shared" si="14"/>
@@ -10950,7 +10770,7 @@
       </c>
       <c r="L84">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70201508619980157</v>
+        <v>0.70059152720545581</v>
       </c>
     </row>
     <row r="85" spans="4:12">
@@ -10960,19 +10780,19 @@
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="9"/>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0957972020903737E-2</v>
+        <v>3.3133639840558997E-2</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="11"/>
-        <v>-11.060156000166982</v>
+        <v>-5.0311405810581045</v>
       </c>
       <c r="I85">
         <f t="shared" ca="1" si="8"/>
-        <v>9.7878378546029304E-29</v>
+        <v>2.4378522859982574E-7</v>
       </c>
       <c r="K85">
         <f t="shared" si="14"/>
@@ -10980,7 +10800,7 @@
       </c>
       <c r="L85">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70214797216952385</v>
+        <v>0.70071926539119156</v>
       </c>
     </row>
     <row r="86" spans="4:12">
@@ -10990,19 +10810,19 @@
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="9"/>
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0768624850057203E-2</v>
+        <v>3.2930985708065387E-2</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="11"/>
-        <v>1.2220240645538634</v>
+        <v>1.6185364286543644</v>
       </c>
       <c r="I86">
         <f t="shared" ca="1" si="8"/>
-        <v>0.88915073658630517</v>
+        <v>0.94722647864545273</v>
       </c>
       <c r="K86">
         <f t="shared" si="14"/>
@@ -11010,7 +10830,7 @@
       </c>
       <c r="L86">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70227962605369476</v>
+        <v>0.70084595362413926</v>
       </c>
     </row>
     <row r="87" spans="4:12">
@@ -11020,19 +10840,19 @@
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="9"/>
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0582710006904334E-2</v>
+        <v>3.2732005120774919E-2</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="11"/>
-        <v>-11.522850653864305</v>
+        <v>-10.592079486751343</v>
       </c>
       <c r="I87">
         <f t="shared" ca="1" si="8"/>
-        <v>5.0603163682771204E-31</v>
+        <v>1.6215306883664949E-26</v>
       </c>
       <c r="K87">
         <f t="shared" si="14"/>
@@ -11040,7 +10860,7 @@
       </c>
       <c r="L87">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70241006311415077</v>
+        <v>0.70097160004934822</v>
       </c>
     </row>
     <row r="88" spans="4:12">
@@ -11050,19 +10870,19 @@
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="9"/>
-        <v>0.12</v>
+        <v>0.91</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0400125031739226E-2</v>
+        <v>3.2536588418307033E-2</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="11"/>
-        <v>-10.605219539834083</v>
+        <v>13.624661390453984</v>
       </c>
       <c r="I88">
         <f t="shared" ca="1" si="8"/>
-        <v>1.4090068865767847E-26</v>
+        <v>1</v>
       </c>
       <c r="K88">
         <f t="shared" si="14"/>
@@ -11070,7 +10890,7 @@
       </c>
       <c r="L88">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70253929863206344</v>
+        <v>0.70109621317735571</v>
       </c>
     </row>
     <row r="89" spans="4:12">
@@ -11080,19 +10900,19 @@
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="9"/>
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0220771696343081E-2</v>
+        <v>3.2344630469149184E-2</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="11"/>
-        <v>8.523938521105709</v>
+        <v>-0.51631444718246688</v>
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0.30281740374032573</v>
       </c>
       <c r="K89">
         <f t="shared" si="14"/>
@@ -11100,7 +10920,7 @@
       </c>
       <c r="L89">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70266734787973606</v>
+        <v>0.70121980183557542</v>
       </c>
     </row>
     <row r="90" spans="4:12">
@@ -11110,19 +10930,19 @@
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="9"/>
-        <v>0.15</v>
+        <v>0.45</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0044555781916539E-2</v>
+        <v>3.2156030432982687E-2</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="11"/>
-        <v>-9.7322124554756169</v>
+        <v>-0.51934271037604873</v>
       </c>
       <c r="I90">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0988013384924939E-22</v>
+        <v>0.30176088719295546</v>
       </c>
       <c r="K90">
         <f t="shared" si="14"/>
@@ -11130,7 +10950,7 @@
       </c>
       <c r="L90">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70279422609564091</v>
+        <v>0.70134237512433917</v>
       </c>
     </row>
     <row r="91" spans="4:12">
@@ -11140,19 +10960,19 @@
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="9"/>
-        <v>0.61</v>
+        <v>0.82</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9871386871091768E-2</v>
+        <v>3.1970691538077828E-2</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="11"/>
-        <v>5.6107204102463664</v>
+        <v>11.050746261750753</v>
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="8"/>
-        <v>0.99999998992569672</v>
+        <v>1</v>
       </c>
       <c r="K91">
         <f t="shared" si="14"/>
@@ -11160,7 +10980,7 @@
       </c>
       <c r="L91">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70291994846235628</v>
+        <v>0.70146394237714393</v>
       </c>
     </row>
     <row r="92" spans="4:12">
@@ -11170,19 +10990,19 @@
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="9"/>
-        <v>0.24</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9701178152981296E-2</v>
+        <v>3.1788520872641876E-2</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="11"/>
-        <v>-6.8145444923936092</v>
+        <v>-12.479347547793942</v>
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="8"/>
-        <v>4.7281452884642813E-12</v>
+        <v>4.8388199489001992E-36</v>
       </c>
       <c r="K92">
         <f t="shared" si="14"/>
@@ -11190,7 +11010,7 @@
       </c>
       <c r="L92">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70304453008711021</v>
+        <v>0.70158451312470582</v>
       </c>
     </row>
     <row r="93" spans="4:12">
@@ -11200,19 +11020,19 @@
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.92</v>
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9533846240308755E-2</v>
+        <v>3.1609429189098127E-2</v>
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="11"/>
-        <v>5.3362504401780999</v>
+        <v>14.340657570505579</v>
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="8"/>
-        <v>0.9999999525558404</v>
+        <v>1</v>
       </c>
       <c r="K93">
         <f t="shared" si="14"/>
@@ -11220,7 +11040,7 @@
       </c>
       <c r="L93">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70316798598466179</v>
+        <v>0.70170409706245684</v>
       </c>
     </row>
     <row r="94" spans="4:12">
@@ -11230,19 +11050,19 @@
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="9"/>
-        <v>0.13</v>
+        <v>0.7</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9369310997746485E-2</v>
+        <v>3.1433330720359406E-2</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="11"/>
-        <v>-10.636953656283275</v>
+        <v>7.4220578810279028</v>
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0029014464211753E-26</v>
+        <v>0.99999999999994238</v>
       </c>
       <c r="K94">
         <f t="shared" si="14"/>
@@ -11250,7 +11070,7 @@
       </c>
       <c r="L94">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70329033106228123</v>
+        <v>0.70182270402116687</v>
       </c>
     </row>
     <row r="95" spans="4:12">
@@ -11260,19 +11080,19 @@
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="9"/>
-        <v>0.31</v>
+        <v>0.46</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9207495380657311E-2</v>
+        <v>3.1260143007236917E-2</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="11"/>
-        <v>-4.5330829732042712</v>
+        <v>-0.21433043343559999</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="8"/>
-        <v>2.9064484150520542E-6</v>
+        <v>0.41514469348564031</v>
       </c>
       <c r="K95">
         <f t="shared" si="14"/>
@@ -11280,7 +11100,7 @@
       </c>
       <c r="L95">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70341158010661797</v>
+        <v>0.70194034394039018</v>
       </c>
     </row>
     <row r="96" spans="4:12">
@@ -11294,15 +11114,15 @@
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9048325283503259E-2</v>
+        <v>3.1089786736195387E-2</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="11"/>
-        <v>0.26163298316946454</v>
+        <v>-0.53715389371125677</v>
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="8"/>
-        <v>0.60319779368955673</v>
+        <v>0.29558065810496503</v>
       </c>
       <c r="K96">
         <f t="shared" si="14"/>
@@ -11310,7 +11130,7 @@
       </c>
       <c r="L96">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7035317477722598</v>
+        <v>0.70205702684448246</v>
       </c>
     </row>
     <row r="97" spans="4:12">
@@ -11320,19 +11140,19 @@
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="9"/>
-        <v>0.28000000000000003</v>
+        <v>0.08</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8891729397243895E-2</v>
+        <v>3.0922185586729673E-2</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="11"/>
-        <v>-5.6209857764863349</v>
+        <v>-12.505584345433627</v>
       </c>
       <c r="I97">
         <f t="shared" ca="1" si="8"/>
-        <v>9.493545327788343E-9</v>
+        <v>3.4793116020267627E-36</v>
       </c>
       <c r="K97">
         <f t="shared" si="14"/>
@@ -11340,7 +11160,7 @@
       </c>
       <c r="L97">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70365084857181392</v>
+        <v>0.70217276282094232</v>
       </c>
     </row>
     <row r="98" spans="4:12">
@@ -11350,19 +11170,19 @@
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="9"/>
-        <v>0.81</v>
+        <v>0.44</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8737639075100848E-2</v>
+        <v>3.0757266087695433E-2</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="11"/>
-        <v>12.791586637974712</v>
+        <v>-0.86808755771311508</v>
       </c>
       <c r="I98">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0.19267320095785612</v>
       </c>
       <c r="K98">
         <f t="shared" si="14"/>
@@ -11370,7 +11190,7 @@
       </c>
       <c r="L98">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70376889686735555</v>
+        <v>0.70228756200086884</v>
       </c>
     </row>
     <row r="99" spans="4:12">
@@ -11380,19 +11200,19 @@
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="9"/>
-        <v>0.48</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8585988206114611E-2</v>
+        <v>3.0594957481979757E-2</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="11"/>
-        <v>1.3153297247900348</v>
+        <v>3.0495221330166329</v>
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="8"/>
-        <v>0.90580044382629898</v>
+        <v>0.99885397128215314</v>
       </c>
       <c r="K99">
         <f t="shared" si="14"/>
@@ -11400,7 +11220,7 @@
       </c>
       <c r="L99">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70388590686310115</v>
+        <v>0.7024014345413373</v>
       </c>
     </row>
     <row r="100" spans="4:12">
@@ -11410,19 +11230,19 @@
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="9"/>
-        <v>0.17</v>
+        <v>0.09</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8436713095964621E-2</v>
+        <v>3.0435191598945498E-2</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="11"/>
-        <v>-9.5791661673674824</v>
+        <v>-12.377119387447905</v>
       </c>
       <c r="I100">
         <f t="shared" ca="1" si="8"/>
-        <v>4.8915776085605554E-22</v>
+        <v>1.7379800306671298E-35</v>
       </c>
       <c r="K100">
         <f t="shared" si="14"/>
@@ -11430,7 +11250,7 @@
       </c>
       <c r="L100">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70400189259918422</v>
+        <v>0.70251439060951959</v>
       </c>
     </row>
     <row r="101" spans="4:12">
@@ -11440,19 +11260,19 @@
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="9"/>
-        <v>0.61</v>
+        <v>0.16</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8289752354564636E-2</v>
+        <v>3.0277902734127071E-2</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="11"/>
-        <v>5.9244067568854897</v>
+        <v>-10.129499479972562</v>
       </c>
       <c r="I101">
         <f t="shared" ref="I101:I104" ca="1" si="15">NORMSDIST(H101)</f>
-        <v>0.99999999843286602</v>
+        <v>2.0436813408305655E-24</v>
       </c>
       <c r="K101">
         <f t="shared" si="14"/>
@@ -11460,7 +11280,7 @@
       </c>
       <c r="L101">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70411686794642081</v>
+        <v>0.70262644036839073</v>
       </c>
     </row>
     <row r="102" spans="4:12">
@@ -11470,19 +11290,19 @@
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="9"/>
-        <v>0.08</v>
+        <v>0.35</v>
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="10"/>
-        <v>2.814504678998285E-2</v>
+        <v>3.012302753569546E-2</v>
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="11"/>
-        <v>-12.876155534727426</v>
+        <v>-3.8741125825321423</v>
       </c>
       <c r="I102">
         <f t="shared" ca="1" si="15"/>
-        <v>3.0657245993009708E-38</v>
+        <v>5.3506967917948955E-5</v>
       </c>
       <c r="K102">
         <f t="shared" si="14"/>
@@ -11490,7 +11310,7 @@
       </c>
       <c r="L102">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70423084660196145</v>
+        <v>0.70273759396387581</v>
       </c>
     </row>
     <row r="103" spans="4:12">
@@ -11500,19 +11320,19 @@
       </c>
       <c r="E103">
         <f t="shared" ca="1" si="9"/>
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
       <c r="G103">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8002539308270416E-2</v>
+        <v>2.9970504897246904E-2</v>
       </c>
       <c r="H103">
         <f t="shared" ca="1" si="11"/>
-        <v>9.9133866734011544</v>
+        <v>-3.5601669163004805</v>
       </c>
       <c r="I103">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v>1.8530957055828967E-4</v>
       </c>
       <c r="K103">
         <f t="shared" si="14"/>
@@ -11520,7 +11340,7 @@
       </c>
       <c r="L103">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7043438420857393</v>
+        <v>0.70284786151330869</v>
       </c>
     </row>
     <row r="104" spans="4:12">
@@ -11530,19 +11350,19 @@
       </c>
       <c r="E104">
         <f t="shared" ca="1" si="9"/>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7862174818813361E-2</v>
+        <v>2.9820275856503098E-2</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.521776396700028</v>
+        <v>-5.590156201175672</v>
       </c>
       <c r="I104">
         <f t="shared" ca="1" si="15"/>
-        <v>6.4032558793492234E-2</v>
+        <v>1.1343272021759342E-8</v>
       </c>
       <c r="K104">
         <f t="shared" si="14"/>
@@ -11550,7 +11370,7 @@
       </c>
       <c r="L104">
         <f t="shared" ca="1" si="12"/>
-        <v>0.70445586773763225</v>
+        <v>0.70295725309508317</v>
       </c>
     </row>
   </sheetData>
@@ -11561,6 +11381,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A6:AP108"/>
   <sheetViews>
     <sheetView topLeftCell="V3" workbookViewId="0">
@@ -16510,160 +16331,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:O19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8">
-        <f>LN(2)+(B9+B10)*LN(B9+B10)+(1-(B9+B10))*LN(1-(B9+B10))</f>
-        <v>2.0135513550688822E-2</v>
-      </c>
-      <c r="E8">
-        <f>EXP(-1*$B$8*D8)</f>
-        <v>0.13351367725131727</v>
-      </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0.5</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9">
-        <f>(B9+B10)*LN((B9+B10)/B9)+(1-(B9+B10))*LN((1-(B9+B10))/(1-B9))</f>
-        <v>2.0135513550688863E-2</v>
-      </c>
-      <c r="E9">
-        <f>EXP(-1*$B$8*D9)</f>
-        <v>0.13351367725131674</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10">
-        <v>0.1</v>
-      </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="G11" s="11"/>
-      <c r="H11" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="7:7">
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>

</xml_diff>